<commit_message>
vendor inventory startup and test script start
</commit_message>
<xml_diff>
--- a/vendors/magic_shop_inventory.xlsx
+++ b/vendors/magic_shop_inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dave_\Documents\DND tool\dnd_random_generation_tools\vendors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE941B66-5FF3-4A93-A8D5-172D8AB06790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B21237D-6714-49A2-B254-7CDE91E69575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7520" yWindow="7280" windowWidth="21470" windowHeight="13700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,67 +25,137 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>copper</t>
+  </si>
+  <si>
+    <t>silver</t>
+  </si>
+  <si>
+    <t>electrum</t>
+  </si>
+  <si>
+    <t>gold</t>
+  </si>
+  <si>
+    <t>platinum</t>
+  </si>
+  <si>
+    <t>Component Pouch</t>
+  </si>
+  <si>
+    <t>Spellbook</t>
+  </si>
+  <si>
+    <t>Arcane Focus: Crystal</t>
+  </si>
+  <si>
+    <t>Arcane Focus: Orb</t>
+  </si>
+  <si>
+    <t>Arcane Focus: Rod</t>
+  </si>
+  <si>
+    <t>Arcane Focus: Staff</t>
+  </si>
+  <si>
+    <t>Arcane Focus: Wand</t>
+  </si>
+  <si>
+    <t>Bottle, glass</t>
+  </si>
+  <si>
+    <t>Candle</t>
+  </si>
+  <si>
+    <t>Case, Map or Scroll</t>
+  </si>
+  <si>
+    <t>Hourglass</t>
+  </si>
+  <si>
+    <t>Quarterstaff</t>
+  </si>
+  <si>
+    <t>Abacus</t>
+  </si>
+  <si>
+    <t>Ink (1 ounce bottle)</t>
+  </si>
+  <si>
+    <t>Ink Pen</t>
+  </si>
+  <si>
+    <t>Paper (one sheet)</t>
+  </si>
+  <si>
+    <t>Parchment (one sheet)</t>
+  </si>
+  <si>
+    <t>Pouch</t>
+  </si>
+  <si>
+    <t>Robes</t>
+  </si>
+  <si>
+    <t>Vial</t>
+  </si>
+  <si>
+    <t>Alchemist's Supplies</t>
+  </si>
+  <si>
+    <t>Calligrapher's Supplies</t>
+  </si>
+  <si>
+    <t>Lute</t>
+  </si>
+  <si>
+    <t>Lyre</t>
+  </si>
+  <si>
+    <t>Druidic Focus: Sprig of Mistletoe</t>
+  </si>
+  <si>
+    <t>Druidic Focus: Totem</t>
+  </si>
+  <si>
+    <t>Druidic Focus: Wooden Staff</t>
+  </si>
+  <si>
+    <t>Druidic Focus: Yew Wand</t>
+  </si>
+  <si>
+    <t>Spell Scroll: Cantrip</t>
+  </si>
+  <si>
+    <t>Spell Scroll: Level 1</t>
+  </si>
+  <si>
+    <t>Spell Scroll: Level 2</t>
+  </si>
+  <si>
+    <t>Spell Scroll: Level 3</t>
+  </si>
+  <si>
+    <t>Spell Scroll: Level 4</t>
+  </si>
+  <si>
+    <t>Spell Scroll: Level 5</t>
+  </si>
   <si>
     <t>Roll</t>
-  </si>
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>copper</t>
-  </si>
-  <si>
-    <t>silver</t>
-  </si>
-  <si>
-    <t>electrum</t>
-  </si>
-  <si>
-    <t>gold</t>
-  </si>
-  <si>
-    <t>platinum</t>
-  </si>
-  <si>
-    <t>Component Pouch</t>
-  </si>
-  <si>
-    <t>Potion of Healing</t>
-  </si>
-  <si>
-    <t>Spellbook</t>
-  </si>
-  <si>
-    <t>Crystal (Arcane Focus)</t>
-  </si>
-  <si>
-    <t>Orb (Arcane Focus)</t>
-  </si>
-  <si>
-    <t>Rod (Arcane Focus)</t>
-  </si>
-  <si>
-    <t>Staff (Arcane Focus)</t>
-  </si>
-  <si>
-    <t>Wand (Arcane Focus)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -113,19 +183,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -407,167 +483,518 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24.81640625" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="6"/>
+    <col min="2" max="2" width="27.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2"/>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="2">
-        <v>10</v>
-      </c>
-      <c r="G2" s="3"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="6"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2">
-        <v>20</v>
-      </c>
-      <c r="G3" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="G3" s="2"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="6"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2">
         <v>10</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="2"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="6"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2">
-        <v>5</v>
-      </c>
-      <c r="G5" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="G5" s="2"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2">
         <v>10</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="2"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="6"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2">
-        <v>25</v>
-      </c>
-      <c r="G7" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="G7" s="2"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="1"/>
+      <c r="F8" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2">
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="1"/>
+      <c r="F9" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="1"/>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="1"/>
+      <c r="F12" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="1"/>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="2"/>
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="2"/>
+      <c r="F15" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="6">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="2"/>
+      <c r="F16" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="6">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="1"/>
+      <c r="F17" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="6">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="1"/>
+      <c r="F18" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="6">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="6">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="6">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="6">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="6">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="1"/>
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="6">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="1"/>
+      <c r="F24" s="2">
         <v>50</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="6">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="1"/>
+      <c r="F25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="6">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="1"/>
+      <c r="F26" s="2">
         <v>50</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="6">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="1"/>
+      <c r="F27" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="6">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="1"/>
+      <c r="F28" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="6">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="1"/>
+      <c r="F29" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="6">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="1"/>
+      <c r="F30" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="6">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="6"/>
+      <c r="D31" s="1"/>
+      <c r="F31" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="6">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="D32" s="1"/>
+      <c r="F32" s="2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="6">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="6"/>
+      <c r="D33" s="1"/>
+      <c r="F33" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="6">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="1"/>
+      <c r="F34" s="2">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="6">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" s="1"/>
+      <c r="F35" s="2">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B36" s="3"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B37" s="3"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>